<commit_message>
Update Report 5/Test Result/DDL_CommonTest Case_v1.0_EN .xlsx
</commit_message>
<xml_diff>
--- a/WIP/Documents/Report 5/Test Result/DDL_CommonTest Case_v1.0_EN .xlsx
+++ b/WIP/Documents/Report 5/Test Result/DDL_CommonTest Case_v1.0_EN .xlsx
@@ -4,44 +4,53 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="821" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="821"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
     <sheet name="Test case List" sheetId="2" r:id="rId2"/>
     <sheet name="Test Report" sheetId="5" r:id="rId3"/>
-    <sheet name="Common" sheetId="14" r:id="rId4"/>
-    <sheet name="Security" sheetId="13" r:id="rId5"/>
-    <sheet name="UI" sheetId="9" r:id="rId6"/>
+    <sheet name="Calculate" sheetId="15" r:id="rId4"/>
+    <sheet name="Common" sheetId="14" r:id="rId5"/>
+    <sheet name="Security" sheetId="13" r:id="rId6"/>
+    <sheet name="UI" sheetId="9" r:id="rId7"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
+    <externalReference r:id="rId9"/>
   </externalReferences>
   <definedNames>
     <definedName name="ACTION" localSheetId="3">#REF!</definedName>
     <definedName name="ACTION" localSheetId="4">#REF!</definedName>
+    <definedName name="ACTION" localSheetId="5">#REF!</definedName>
     <definedName name="ACTION">#REF!</definedName>
     <definedName name="d">'[1]Search grammar'!$C$45</definedName>
     <definedName name="Defect" comment="fsfsdfs" localSheetId="3">#REF!</definedName>
     <definedName name="Defect" comment="fsfsdfs" localSheetId="4">#REF!</definedName>
+    <definedName name="Defect" comment="fsfsdfs" localSheetId="5">#REF!</definedName>
     <definedName name="Defect" comment="fsfsdfs">#REF!</definedName>
     <definedName name="dfsf" localSheetId="3">#REF!</definedName>
     <definedName name="dfsf" localSheetId="4">#REF!</definedName>
+    <definedName name="dfsf" localSheetId="5">#REF!</definedName>
     <definedName name="dfsf">#REF!</definedName>
     <definedName name="Discover" localSheetId="3">#REF!</definedName>
     <definedName name="Discover" localSheetId="4">#REF!</definedName>
+    <definedName name="Discover" localSheetId="5">#REF!</definedName>
     <definedName name="Discover">#REF!</definedName>
     <definedName name="Lỗi" localSheetId="3">#REF!</definedName>
     <definedName name="Lỗi" localSheetId="4">#REF!</definedName>
+    <definedName name="Lỗi" localSheetId="5">#REF!</definedName>
     <definedName name="Lỗi">#REF!</definedName>
     <definedName name="Pass" localSheetId="3">#REF!</definedName>
     <definedName name="Pass" localSheetId="4">#REF!</definedName>
+    <definedName name="Pass" localSheetId="5">#REF!</definedName>
     <definedName name="Pass">#REF!</definedName>
     <definedName name="Statistic" comment="fsfsdfs" localSheetId="3">#REF!</definedName>
     <definedName name="Statistic" comment="fsfsdfs" localSheetId="4">#REF!</definedName>
+    <definedName name="Statistic" comment="fsfsdfs" localSheetId="5">#REF!</definedName>
     <definedName name="Statistic" comment="fsfsdfs">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="145621" iterate="1" iterateCount="10000" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="144525" iterate="1" iterateCount="10000" iterateDelta="1.0000000000000001E-5"/>
 </workbook>
 </file>
 
@@ -203,6 +212,88 @@
         </r>
       </text>
     </comment>
+    <comment ref="J10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Chinh Vu Cong:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+ManhNL
+HuyNM
+AnhDD
+TrungVN
+ChinhVC
+MaiCTP</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tester:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ChinhVC
+MaiCTP</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Status:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Open
+Accepted
+Ready for test
+Close
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -247,12 +338,94 @@
         </r>
       </text>
     </comment>
+    <comment ref="J10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Chinh Vu Cong:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+ManhNL
+HuyNM
+AnhDD
+TrungVN
+ChinhVC
+MaiCTP</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tester:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ChinhVC
+MaiCTP</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Status:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Open
+Accepted
+Ready for test
+Close
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="169">
   <si>
     <t>TEST CASE</t>
   </si>
@@ -773,15 +946,76 @@
   <si>
     <t>Check width of browser &gt;= 800x600  px</t>
   </si>
+  <si>
+    <t>Defects</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>STATUS</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>Accepted</t>
+  </si>
+  <si>
+    <t>Ready for Test</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>∑</t>
+  </si>
+  <si>
+    <t>ChinhVC</t>
+  </si>
+  <si>
+    <t>Developer</t>
+  </si>
+  <si>
+    <t>ManhNL</t>
+  </si>
+  <si>
+    <t>HuyNM</t>
+  </si>
+  <si>
+    <t>AnhDD</t>
+  </si>
+  <si>
+    <t>TrungVN</t>
+  </si>
+  <si>
+    <t>Empty</t>
+  </si>
+  <si>
+    <t>Assignee</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Open Date</t>
+  </si>
+  <si>
+    <t>Close Date</t>
+  </si>
+  <si>
+    <t>Evident</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d\-mmm\-yy;@"/>
+    <numFmt numFmtId="165" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="32">
     <font>
       <sz val="11"/>
       <name val="ＭＳ Ｐゴシック"/>
@@ -952,8 +1186,46 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -990,8 +1262,44 @@
         <bgColor indexed="26"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="32"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="26"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66FFFF"/>
+        <bgColor indexed="41"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="26"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="35">
+  <borders count="53">
     <border>
       <left/>
       <right/>
@@ -1471,6 +1779,256 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1482,7 +2040,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="149">
+  <cellXfs count="195">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1828,9 +2386,6 @@
     <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="33" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="34" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1876,6 +2431,135 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="27" fillId="7" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="26" fillId="7" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="27" fillId="8" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="1" fontId="26" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="27" fillId="8" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="1" fontId="26" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="27" fillId="8" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="165" fontId="26" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="27" fillId="7" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="45" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="46" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="47" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="21" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="9" borderId="21" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="10" borderId="21" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="52" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="12" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="21" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="26" fillId="6" borderId="21" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="3" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="3" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="3" borderId="14" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="21" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="9" borderId="21" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="10" borderId="21" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="32" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="34" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="11" borderId="52" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="26" fillId="12" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="33" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1979,6 +2663,31 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Cover"/>
+      <sheetName val="Test case List"/>
+      <sheetName val="Test Report"/>
+      <sheetName val="Calculate"/>
+      <sheetName val="Message Rules"/>
+      <sheetName val="User_Function"/>
+      <sheetName val="Admin_Function"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2334,8 +3043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2353,13 +3062,13 @@
     <row r="2" spans="1:7" s="5" customFormat="1" ht="75.75" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="134" t="s">
+      <c r="C2" s="133" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="134"/>
-      <c r="E2" s="134"/>
-      <c r="F2" s="134"/>
-      <c r="G2" s="134"/>
+      <c r="D2" s="133"/>
+      <c r="E2" s="133"/>
+      <c r="F2" s="133"/>
+      <c r="G2" s="133"/>
     </row>
     <row r="3" spans="1:7">
       <c r="B3" s="6"/>
@@ -2370,11 +3079,11 @@
       <c r="B4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="135" t="s">
+      <c r="C4" s="134" t="s">
         <v>57</v>
       </c>
-      <c r="D4" s="135"/>
-      <c r="E4" s="135"/>
+      <c r="D4" s="134"/>
+      <c r="E4" s="134"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
@@ -2386,11 +3095,11 @@
       <c r="B5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="135" t="s">
+      <c r="C5" s="134" t="s">
         <v>58</v>
       </c>
-      <c r="D5" s="135"/>
-      <c r="E5" s="135"/>
+      <c r="D5" s="134"/>
+      <c r="E5" s="134"/>
       <c r="F5" s="9" t="s">
         <v>4</v>
       </c>
@@ -2399,15 +3108,15 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B6" s="136" t="s">
+      <c r="B6" s="135" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="137" t="str">
+      <c r="C6" s="136" t="str">
         <f>C5&amp;"_"&amp;"Common Test Case"&amp;"_"&amp;"v1.0"</f>
         <v>DDL_Common Test Case_v1.0</v>
       </c>
-      <c r="D6" s="137"/>
-      <c r="E6" s="137"/>
+      <c r="D6" s="136"/>
+      <c r="E6" s="136"/>
       <c r="F6" s="9" t="s">
         <v>6</v>
       </c>
@@ -2416,10 +3125,10 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="13.5" customHeight="1">
-      <c r="B7" s="136"/>
-      <c r="C7" s="137"/>
-      <c r="D7" s="137"/>
-      <c r="E7" s="137"/>
+      <c r="B7" s="135"/>
+      <c r="C7" s="136"/>
+      <c r="D7" s="136"/>
+      <c r="E7" s="136"/>
       <c r="F7" s="9" t="s">
         <v>7</v>
       </c>
@@ -2581,39 +3290,39 @@
       <c r="E2" s="34"/>
     </row>
     <row r="3" spans="2:6">
-      <c r="B3" s="140" t="s">
+      <c r="B3" s="139" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="140"/>
-      <c r="D3" s="141" t="str">
+      <c r="C3" s="139"/>
+      <c r="D3" s="140" t="str">
         <f>Cover!C4</f>
         <v>Dandelion</v>
       </c>
-      <c r="E3" s="141"/>
-      <c r="F3" s="141"/>
+      <c r="E3" s="140"/>
+      <c r="F3" s="140"/>
     </row>
     <row r="4" spans="2:6">
-      <c r="B4" s="140" t="s">
+      <c r="B4" s="139" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="140"/>
-      <c r="D4" s="141" t="str">
+      <c r="C4" s="139"/>
+      <c r="D4" s="140" t="str">
         <f>Cover!C5</f>
         <v>DDL</v>
       </c>
-      <c r="E4" s="141"/>
-      <c r="F4" s="141"/>
+      <c r="E4" s="140"/>
+      <c r="F4" s="140"/>
     </row>
     <row r="5" spans="2:6" s="35" customFormat="1" ht="72" customHeight="1">
-      <c r="B5" s="138" t="s">
+      <c r="B5" s="137" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="138"/>
-      <c r="D5" s="139" t="s">
+      <c r="C5" s="137"/>
+      <c r="D5" s="138" t="s">
         <v>59</v>
       </c>
-      <c r="E5" s="139"/>
-      <c r="F5" s="139"/>
+      <c r="E5" s="138"/>
+      <c r="F5" s="138"/>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="36"/>
@@ -2776,8 +3485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2791,15 +3500,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25.5" customHeight="1">
-      <c r="B1" s="144" t="s">
+      <c r="B1" s="143" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="144"/>
-      <c r="D1" s="144"/>
-      <c r="E1" s="144"/>
-      <c r="F1" s="144"/>
-      <c r="G1" s="144"/>
-      <c r="H1" s="144"/>
+      <c r="C1" s="143"/>
+      <c r="D1" s="143"/>
+      <c r="E1" s="143"/>
+      <c r="F1" s="143"/>
+      <c r="G1" s="143"/>
+      <c r="H1" s="143"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" customHeight="1">
       <c r="A2" s="58"/>
@@ -2815,15 +3524,15 @@
       <c r="B3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="141" t="str">
+      <c r="C3" s="140" t="str">
         <f>Cover!C4</f>
         <v>Dandelion</v>
       </c>
-      <c r="D3" s="141"/>
-      <c r="E3" s="142" t="s">
+      <c r="D3" s="140"/>
+      <c r="E3" s="141" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="142"/>
+      <c r="F3" s="141"/>
       <c r="G3" s="10" t="s">
         <v>64</v>
       </c>
@@ -2833,15 +3542,15 @@
       <c r="B4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="141" t="str">
+      <c r="C4" s="140" t="str">
         <f>Cover!C5</f>
         <v>DDL</v>
       </c>
-      <c r="D4" s="141"/>
-      <c r="E4" s="142" t="s">
+      <c r="D4" s="140"/>
+      <c r="E4" s="141" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="142"/>
+      <c r="F4" s="141"/>
       <c r="G4" s="10" t="s">
         <v>128</v>
       </c>
@@ -2851,15 +3560,15 @@
       <c r="B5" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="141" t="str">
+      <c r="C5" s="140" t="str">
         <f>C4&amp;"_"&amp;"Integration Test Report"&amp;"_"&amp;"v1.0"</f>
         <v>DDL_Integration Test Report_v1.0</v>
       </c>
-      <c r="D5" s="141"/>
-      <c r="E5" s="142" t="s">
+      <c r="D5" s="140"/>
+      <c r="E5" s="141" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="142"/>
+      <c r="F5" s="141"/>
       <c r="G5" s="104"/>
       <c r="H5" s="63"/>
     </row>
@@ -2868,12 +3577,12 @@
       <c r="B6" s="62" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="143"/>
-      <c r="D6" s="143"/>
-      <c r="E6" s="143"/>
-      <c r="F6" s="143"/>
-      <c r="G6" s="143"/>
-      <c r="H6" s="143"/>
+      <c r="C6" s="142"/>
+      <c r="D6" s="142"/>
+      <c r="E6" s="142"/>
+      <c r="F6" s="142"/>
+      <c r="G6" s="142"/>
+      <c r="H6" s="142"/>
     </row>
     <row r="7" spans="1:8" ht="14.25" customHeight="1">
       <c r="A7" s="58"/>
@@ -3116,11 +3825,335 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:F21"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9" style="148"/>
+    <col min="2" max="2" width="12.375" style="148" customWidth="1"/>
+    <col min="3" max="3" width="9" style="148" customWidth="1"/>
+    <col min="4" max="4" width="13.375" style="148" customWidth="1"/>
+    <col min="5" max="6" width="9" style="148" customWidth="1"/>
+    <col min="7" max="7" width="13" style="148" customWidth="1"/>
+    <col min="8" max="8" width="14.25" style="148" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="148"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1"/>
+    <row r="3" spans="1:6" ht="15.75" thickBot="1">
+      <c r="B3" s="149" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3" s="150" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15" customHeight="1">
+      <c r="A4" s="151" t="s">
+        <v>151</v>
+      </c>
+      <c r="B4" s="152" t="s">
+        <v>152</v>
+      </c>
+      <c r="C4" s="153">
+        <f>Security!J8 + UI!J8</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="154"/>
+      <c r="B5" s="155" t="s">
+        <v>153</v>
+      </c>
+      <c r="C5" s="156">
+        <f>Security!K8 + UI!K8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="154"/>
+      <c r="B6" s="155" t="s">
+        <v>154</v>
+      </c>
+      <c r="C6" s="156">
+        <f>Security!L8 + UI!L8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="154"/>
+      <c r="B7" s="155" t="s">
+        <v>155</v>
+      </c>
+      <c r="C7" s="156">
+        <f>Security!M8 + UI!M8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A8" s="157"/>
+      <c r="B8" s="158" t="s">
+        <v>156</v>
+      </c>
+      <c r="C8" s="159">
+        <f>SUM(C4:C7)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="160"/>
+      <c r="B9" s="160"/>
+      <c r="C9" s="160"/>
+      <c r="D9" s="160"/>
+      <c r="E9" s="160"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="161" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="162"/>
+      <c r="C10" s="162"/>
+      <c r="D10" s="163"/>
+      <c r="E10" s="160"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="164" t="s">
+        <v>157</v>
+      </c>
+      <c r="B11" s="162"/>
+      <c r="C11" s="162"/>
+      <c r="D11" s="165"/>
+      <c r="E11" s="160"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="164" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="162"/>
+      <c r="C12" s="162"/>
+      <c r="D12" s="165"/>
+      <c r="E12" s="160"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="B13" s="162"/>
+      <c r="C13" s="162"/>
+      <c r="D13" s="165"/>
+      <c r="E13" s="160"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="161" t="s">
+        <v>158</v>
+      </c>
+      <c r="B14" s="161" t="s">
+        <v>152</v>
+      </c>
+      <c r="C14" s="161" t="s">
+        <v>153</v>
+      </c>
+      <c r="D14" s="161" t="s">
+        <v>154</v>
+      </c>
+      <c r="E14" s="161" t="s">
+        <v>155</v>
+      </c>
+      <c r="F14" s="161" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="164" t="s">
+        <v>159</v>
+      </c>
+      <c r="B15" s="164">
+        <f>Security!J2 + UI!J2</f>
+        <v>0</v>
+      </c>
+      <c r="C15" s="164">
+        <f>Security!K2 + UI!K2</f>
+        <v>0</v>
+      </c>
+      <c r="D15" s="164">
+        <f>Security!L2 + UI!L2</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="164">
+        <f>Security!M2 + UI!M2</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="166">
+        <f t="shared" ref="F15:F20" si="0">SUM(B15:E15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="164" t="s">
+        <v>160</v>
+      </c>
+      <c r="B16" s="164">
+        <f>Security!J3 + UI!J3</f>
+        <v>0</v>
+      </c>
+      <c r="C16" s="164">
+        <f>Security!K3 + UI!K3</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="164">
+        <f>Security!L3 + UI!L3</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="164">
+        <f>Security!M3 + UI!M3</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="166">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="164" t="s">
+        <v>161</v>
+      </c>
+      <c r="B17" s="164">
+        <f>Security!J4 + UI!J4</f>
+        <v>0</v>
+      </c>
+      <c r="C17" s="164">
+        <f>Security!K4 + UI!K4</f>
+        <v>0</v>
+      </c>
+      <c r="D17" s="164">
+        <f>Security!L4 + UI!L4</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="164">
+        <f>Security!M4 + UI!M4</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="166">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="164" t="s">
+        <v>162</v>
+      </c>
+      <c r="B18" s="164">
+        <f>Security!J5 + UI!J5</f>
+        <v>1</v>
+      </c>
+      <c r="C18" s="164">
+        <f>Security!K5 + UI!K5</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="164">
+        <f>Security!L5 + UI!L5</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="164">
+        <f>Security!M5 + UI!M5</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="166">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="164" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="164">
+        <f>Security!J6 + UI!J6</f>
+        <v>0</v>
+      </c>
+      <c r="C19" s="164">
+        <f>Security!K6 + UI!K6</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="164">
+        <f>Security!L6 + UI!L6</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="164">
+        <f>Security!M6 + UI!M6</f>
+        <v>0</v>
+      </c>
+      <c r="F19" s="166">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="164" t="s">
+        <v>157</v>
+      </c>
+      <c r="B20" s="164">
+        <f>Security!J7 + UI!J7</f>
+        <v>0</v>
+      </c>
+      <c r="C20" s="164">
+        <f>Security!K7 + UI!K7</f>
+        <v>0</v>
+      </c>
+      <c r="D20" s="164">
+        <f>Security!L7 + UI!L7</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="164">
+        <f>Security!M7 + UI!M7</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="166">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="166" t="s">
+        <v>156</v>
+      </c>
+      <c r="B21" s="166">
+        <f>SUM(B15:B20)</f>
+        <v>1</v>
+      </c>
+      <c r="C21" s="166">
+        <f>SUM(C15:C20)</f>
+        <v>0</v>
+      </c>
+      <c r="D21" s="166">
+        <f>SUM(D15:D20)</f>
+        <v>0</v>
+      </c>
+      <c r="E21" s="166">
+        <f>SUM(E15:E20)</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="166">
+        <f>SUM(F15:F20)</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A4:A8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IW17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12:H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.25" defaultRowHeight="13.5" customHeight="1"/>
@@ -3399,14 +4432,14 @@
       <c r="A2" s="111" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="145" t="s">
+      <c r="B2" s="144" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="145"/>
-      <c r="D2" s="145"/>
-      <c r="E2" s="145"/>
-      <c r="F2" s="145"/>
-      <c r="G2" s="145"/>
+      <c r="C2" s="144"/>
+      <c r="D2" s="144"/>
+      <c r="E2" s="144"/>
+      <c r="F2" s="144"/>
+      <c r="G2" s="144"/>
       <c r="H2" s="118" t="s">
         <v>22</v>
       </c>
@@ -3659,14 +4692,14 @@
       <c r="A3" s="112" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="145" t="s">
+      <c r="B3" s="144" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="145"/>
-      <c r="D3" s="145"/>
-      <c r="E3" s="145"/>
-      <c r="F3" s="145"/>
-      <c r="G3" s="145"/>
+      <c r="C3" s="144"/>
+      <c r="D3" s="144"/>
+      <c r="E3" s="144"/>
+      <c r="F3" s="144"/>
+      <c r="G3" s="144"/>
       <c r="H3" s="118" t="s">
         <v>24</v>
       </c>
@@ -3919,14 +4952,14 @@
       <c r="A4" s="111" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="146" t="s">
+      <c r="B4" s="145" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="146"/>
-      <c r="D4" s="146"/>
-      <c r="E4" s="146"/>
-      <c r="F4" s="146"/>
-      <c r="G4" s="146"/>
+      <c r="C4" s="145"/>
+      <c r="D4" s="145"/>
+      <c r="E4" s="145"/>
+      <c r="F4" s="145"/>
+      <c r="G4" s="145"/>
       <c r="H4" s="118" t="s">
         <v>27</v>
       </c>
@@ -4186,11 +5219,11 @@
       <c r="D5" s="92" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="147" t="s">
+      <c r="E5" s="146" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="147"/>
-      <c r="G5" s="147"/>
+      <c r="F5" s="146"/>
+      <c r="G5" s="146"/>
       <c r="H5" s="119" t="s">
         <v>26</v>
       </c>
@@ -4456,12 +5489,12 @@
         <f>COUNTIF(F11:G623,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="148">
+      <c r="E6" s="147">
         <f>COUNTA(A11:A180)*2</f>
         <v>12</v>
       </c>
-      <c r="F6" s="148"/>
-      <c r="G6" s="148"/>
+      <c r="F6" s="147"/>
+      <c r="G6" s="147"/>
       <c r="H6" s="93"/>
       <c r="I6" s="89"/>
       <c r="J6" s="89" t="s">
@@ -5948,12 +6981,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IW22"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B20" sqref="A19:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.25" defaultRowHeight="13.5" customHeight="1"/>
@@ -5967,14 +7000,14 @@
     <col min="7" max="7" width="13.25" style="98" customWidth="1"/>
     <col min="8" max="8" width="15.25" style="100" customWidth="1"/>
     <col min="9" max="9" width="15.25" style="98" customWidth="1"/>
-    <col min="10" max="10" width="13.875" style="99" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="13.875" style="99" customWidth="1"/>
     <col min="11" max="11" width="15.25" style="98" customWidth="1"/>
     <col min="12" max="16" width="15.25" style="98"/>
     <col min="17" max="17" width="0" style="98" hidden="1" customWidth="1"/>
     <col min="18" max="16384" width="15.25" style="98"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:257" ht="13.5" customHeight="1" thickBot="1">
+    <row r="1" spans="1:257" ht="13.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A1" s="110" t="s">
         <v>48</v>
       </c>
@@ -5985,13 +7018,27 @@
       <c r="F1" s="86"/>
       <c r="G1" s="87"/>
       <c r="H1" s="88"/>
-      <c r="I1" s="89"/>
-      <c r="J1" s="89"/>
-      <c r="K1" s="89"/>
-      <c r="L1" s="89"/>
-      <c r="M1" s="89"/>
-      <c r="N1" s="89"/>
-      <c r="O1" s="89"/>
+      <c r="I1" s="167" t="s">
+        <v>158</v>
+      </c>
+      <c r="J1" s="168" t="s">
+        <v>152</v>
+      </c>
+      <c r="K1" s="168" t="s">
+        <v>153</v>
+      </c>
+      <c r="L1" s="168" t="s">
+        <v>154</v>
+      </c>
+      <c r="M1" s="168" t="s">
+        <v>155</v>
+      </c>
+      <c r="N1" s="168" t="s">
+        <v>163</v>
+      </c>
+      <c r="O1" s="169" t="s">
+        <v>150</v>
+      </c>
       <c r="P1" s="89"/>
       <c r="Q1" s="89"/>
       <c r="R1" s="89"/>
@@ -6232,26 +7279,44 @@
       <c r="A2" s="111" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="145" t="s">
+      <c r="B2" s="144" t="s">
         <v>80</v>
       </c>
-      <c r="C2" s="145"/>
-      <c r="D2" s="145"/>
-      <c r="E2" s="145"/>
-      <c r="F2" s="145"/>
-      <c r="G2" s="145"/>
+      <c r="C2" s="144"/>
+      <c r="D2" s="144"/>
+      <c r="E2" s="144"/>
+      <c r="F2" s="144"/>
+      <c r="G2" s="144"/>
       <c r="H2" s="118" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
-      <c r="O2" s="89"/>
+      <c r="I2" s="170" t="s">
+        <v>159</v>
+      </c>
+      <c r="J2" s="164">
+        <f>COUNTIFS(J12:J137,"ManhNL",L12:L137,"Open")</f>
+        <v>0</v>
+      </c>
+      <c r="K2" s="164">
+        <f>COUNTIFS(J12:J137,"ManhNL",L12:L137,"Accepted")</f>
+        <v>0</v>
+      </c>
+      <c r="L2" s="164">
+        <f>COUNTIFS(J12:J137,"ManhNL",L12:L137,"Ready for test")</f>
+        <v>0</v>
+      </c>
+      <c r="M2" s="164">
+        <f>COUNTIFS(J12:J137,"ManhNL",L12:L137,"Closed")</f>
+        <v>0</v>
+      </c>
+      <c r="N2" s="164">
+        <f>COUNTIFS(J12:J137,"ManhNL",L12:L137,"")</f>
+        <v>0</v>
+      </c>
+      <c r="O2" s="171">
+        <f t="shared" ref="O2:O7" si="0">SUM(J2:N2)</f>
+        <v>0</v>
+      </c>
       <c r="P2" s="89"/>
       <c r="Q2" s="89"/>
       <c r="R2" s="89"/>
@@ -6492,26 +7557,44 @@
       <c r="A3" s="112" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="145" t="s">
+      <c r="B3" s="144" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="145"/>
-      <c r="D3" s="145"/>
-      <c r="E3" s="145"/>
-      <c r="F3" s="145"/>
-      <c r="G3" s="145"/>
+      <c r="C3" s="144"/>
+      <c r="D3" s="144"/>
+      <c r="E3" s="144"/>
+      <c r="F3" s="144"/>
+      <c r="G3" s="144"/>
       <c r="H3" s="118" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
-      <c r="O3" s="89"/>
+      <c r="I3" s="170" t="s">
+        <v>160</v>
+      </c>
+      <c r="J3" s="164">
+        <f>COUNTIFS(J12:J137,"HuyNM",L12:L137,"Open")</f>
+        <v>0</v>
+      </c>
+      <c r="K3" s="164">
+        <f>COUNTIFS(J12:J137,"HuyNM",L12:L137,"Accepted")</f>
+        <v>0</v>
+      </c>
+      <c r="L3" s="164">
+        <f>COUNTIFS(J12:J137,"HuyNM",L12:L137,"Ready for test")</f>
+        <v>0</v>
+      </c>
+      <c r="M3" s="164">
+        <f>COUNTIFS(J12:J137,"HuyNM",L12:L137,"Closed")</f>
+        <v>0</v>
+      </c>
+      <c r="N3" s="164">
+        <f>COUNTIFS(J12:J137,"HuyNM",L12:L137,"")</f>
+        <v>0</v>
+      </c>
+      <c r="O3" s="172">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="P3" s="89"/>
       <c r="Q3" s="89"/>
       <c r="R3" s="89"/>
@@ -6752,24 +7835,44 @@
       <c r="A4" s="111" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="146" t="s">
+      <c r="B4" s="145" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="146"/>
-      <c r="D4" s="146"/>
-      <c r="E4" s="146"/>
-      <c r="F4" s="146"/>
-      <c r="G4" s="146"/>
+      <c r="C4" s="145"/>
+      <c r="D4" s="145"/>
+      <c r="E4" s="145"/>
+      <c r="F4" s="145"/>
+      <c r="G4" s="145"/>
       <c r="H4" s="118" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="89"/>
-      <c r="J4" s="90"/>
-      <c r="K4" s="89"/>
-      <c r="L4" s="89"/>
-      <c r="M4" s="89"/>
-      <c r="N4" s="89"/>
-      <c r="O4" s="89"/>
+      <c r="I4" s="170" t="s">
+        <v>161</v>
+      </c>
+      <c r="J4" s="164">
+        <f>COUNTIFS(J12:J137,"AnhDD",L12:L137,"Open")</f>
+        <v>0</v>
+      </c>
+      <c r="K4" s="164">
+        <f>COUNTIFS(J12:J137,"AnhDD",L12:L137,"Accepted")</f>
+        <v>0</v>
+      </c>
+      <c r="L4" s="164">
+        <f>COUNTIFS(J12:J137,"AnhDD",L12:L137,"Ready for test")</f>
+        <v>0</v>
+      </c>
+      <c r="M4" s="164">
+        <f>COUNTIFS(J12:J137,"AnhDD",L12:L137,"Closed")</f>
+        <v>0</v>
+      </c>
+      <c r="N4" s="164">
+        <f>COUNTIFS(J12:J137,"AnhDD",L12:L137,"")</f>
+        <v>0</v>
+      </c>
+      <c r="O4" s="172">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="P4" s="89"/>
       <c r="Q4" s="89"/>
       <c r="R4" s="89"/>
@@ -7019,23 +8122,41 @@
       <c r="D5" s="92" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="147" t="s">
+      <c r="E5" s="146" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="147"/>
-      <c r="G5" s="147"/>
+      <c r="F5" s="146"/>
+      <c r="G5" s="146"/>
       <c r="H5" s="119" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="89"/>
-      <c r="J5" s="89" t="s">
-        <v>29</v>
-      </c>
-      <c r="K5" s="89"/>
-      <c r="L5" s="89"/>
-      <c r="M5" s="89"/>
-      <c r="N5" s="89"/>
-      <c r="O5" s="89"/>
+      <c r="I5" s="170" t="s">
+        <v>162</v>
+      </c>
+      <c r="J5" s="164">
+        <f>COUNTIFS(J12:J137,"TrungVN",L12:L137,"Open")</f>
+        <v>1</v>
+      </c>
+      <c r="K5" s="164">
+        <f>COUNTIFS(J12:J137,"TrungVN",L12:L137,"Accepted")</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="164">
+        <f>COUNTIFS(J12:J137,"TrungVN",L12:L137,"Ready for test")</f>
+        <v>0</v>
+      </c>
+      <c r="M5" s="164">
+        <f>COUNTIFS(J12:J137,"TrungVN",L12:L137,"Closed")</f>
+        <v>0</v>
+      </c>
+      <c r="N5" s="164">
+        <f>COUNTIFS(J12:J137,"TrungVN",L12:L137,"")</f>
+        <v>0</v>
+      </c>
+      <c r="O5" s="172">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="P5" s="89"/>
       <c r="Q5" s="89"/>
       <c r="R5" s="89"/>
@@ -7289,22 +8410,40 @@
         <f>COUNTIF(F11:G628,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="148">
+      <c r="E6" s="147">
         <f>COUNTA(A11:A185)*2</f>
         <v>20</v>
       </c>
-      <c r="F6" s="148"/>
-      <c r="G6" s="148"/>
+      <c r="F6" s="147"/>
+      <c r="G6" s="147"/>
       <c r="H6" s="93"/>
-      <c r="I6" s="89"/>
-      <c r="J6" s="89" t="s">
-        <v>27</v>
-      </c>
-      <c r="K6" s="89"/>
-      <c r="L6" s="89"/>
-      <c r="M6" s="89"/>
-      <c r="N6" s="89"/>
-      <c r="O6" s="89"/>
+      <c r="I6" s="170" t="s">
+        <v>64</v>
+      </c>
+      <c r="J6" s="164">
+        <f>COUNTIFS(J12:J137,"MaiCTP",L12:L137,"Open")</f>
+        <v>0</v>
+      </c>
+      <c r="K6" s="164">
+        <f>COUNTIFS(J12:J137,"MaiCTP",L12:L137,"Accepted")</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="164">
+        <f>COUNTIFS(J12:J137,"MaiCTP",L12:L137,"Ready for test")</f>
+        <v>0</v>
+      </c>
+      <c r="M6" s="164">
+        <f>COUNTIFS(J12:J137,"MaiCTP",L12:L137,"Closed")</f>
+        <v>0</v>
+      </c>
+      <c r="N6" s="164">
+        <f>COUNTIFS(J12:J137,"MaiCTP",L12:L137,"")</f>
+        <v>0</v>
+      </c>
+      <c r="O6" s="172">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="P6" s="89"/>
       <c r="Q6" s="89"/>
       <c r="R6" s="89"/>
@@ -7550,13 +8689,33 @@
       <c r="F7" s="131"/>
       <c r="G7" s="131"/>
       <c r="H7" s="93"/>
-      <c r="I7" s="89"/>
-      <c r="J7" s="89"/>
-      <c r="K7" s="89"/>
-      <c r="L7" s="89"/>
-      <c r="M7" s="89"/>
-      <c r="N7" s="89"/>
-      <c r="O7" s="89"/>
+      <c r="I7" s="170" t="s">
+        <v>157</v>
+      </c>
+      <c r="J7" s="164">
+        <f>COUNTIFS(J12:J137,"ChinhVC",L12:L137,"Open")</f>
+        <v>0</v>
+      </c>
+      <c r="K7" s="164">
+        <f>COUNTIFS(J12:J137,"ChinhVC",L12:L137,"Accepted")</f>
+        <v>0</v>
+      </c>
+      <c r="L7" s="164">
+        <f>COUNTIFS(J12:J137,"ChinhVC",L12:L137,"Ready for test")</f>
+        <v>0</v>
+      </c>
+      <c r="M7" s="164">
+        <f>COUNTIFS(J12:J137,"ChinhVC",L12:L137,"Closed")</f>
+        <v>0</v>
+      </c>
+      <c r="N7" s="164">
+        <f>COUNTIFS(J12:J137,"ChinhVC",L12:L137,"")</f>
+        <v>0</v>
+      </c>
+      <c r="O7" s="172">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="P7" s="89"/>
       <c r="Q7" s="89"/>
       <c r="R7" s="89"/>
@@ -7793,7 +8952,7 @@
       <c r="IO7" s="89"/>
       <c r="IP7" s="89"/>
     </row>
-    <row r="8" spans="1:257" ht="13.5" customHeight="1">
+    <row r="8" spans="1:257" ht="13.5" customHeight="1" thickBot="1">
       <c r="A8" s="129"/>
       <c r="B8" s="130"/>
       <c r="C8" s="130"/>
@@ -7802,13 +8961,33 @@
       <c r="F8" s="131"/>
       <c r="G8" s="131"/>
       <c r="H8" s="93"/>
-      <c r="I8" s="89"/>
-      <c r="J8" s="89"/>
-      <c r="K8" s="89"/>
-      <c r="L8" s="89"/>
-      <c r="M8" s="89"/>
-      <c r="N8" s="89"/>
-      <c r="O8" s="89"/>
+      <c r="I8" s="173" t="s">
+        <v>156</v>
+      </c>
+      <c r="J8" s="174">
+        <f>SUM(J2:J7)</f>
+        <v>1</v>
+      </c>
+      <c r="K8" s="174">
+        <f t="shared" ref="K8:O8" si="1">SUM(K2:K7)</f>
+        <v>0</v>
+      </c>
+      <c r="L8" s="174">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M8" s="174">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N8" s="174">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O8" s="174">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
       <c r="P8" s="89"/>
       <c r="Q8" s="89"/>
       <c r="R8" s="89"/>
@@ -8045,7 +9224,7 @@
       <c r="IO8" s="89"/>
       <c r="IP8" s="89"/>
     </row>
-    <row r="9" spans="1:257" ht="13.5" customHeight="1">
+    <row r="9" spans="1:257" ht="13.5" customHeight="1" thickTop="1">
       <c r="A9" s="115"/>
       <c r="B9" s="89"/>
       <c r="C9" s="89"/>
@@ -8304,41 +9483,52 @@
       <c r="IV9" s="89"/>
       <c r="IW9" s="89"/>
     </row>
-    <row r="10" spans="1:257" ht="36" customHeight="1">
-      <c r="A10" s="116" t="s">
+    <row r="10" spans="1:257" ht="39.75" customHeight="1">
+      <c r="A10" s="183" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="184" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="56" t="s">
+      <c r="C10" s="184" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="56" t="s">
+      <c r="D10" s="184" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="57" t="s">
+      <c r="E10" s="185" t="s">
         <v>34</v>
       </c>
-      <c r="F10" s="57" t="s">
+      <c r="F10" s="185" t="s">
         <v>62</v>
       </c>
-      <c r="G10" s="57" t="s">
+      <c r="G10" s="185" t="s">
         <v>63</v>
       </c>
-      <c r="H10" s="57" t="s">
+      <c r="H10" s="185" t="s">
         <v>35</v>
       </c>
-      <c r="I10" s="56" t="s">
+      <c r="I10" s="184" t="s">
         <v>36</v>
       </c>
-      <c r="J10" s="89"/>
-      <c r="K10" s="89"/>
-      <c r="L10" s="89"/>
-      <c r="M10" s="89"/>
-      <c r="N10" s="89"/>
-      <c r="O10" s="89"/>
-      <c r="P10" s="89"/>
+      <c r="J10" s="186" t="s">
+        <v>164</v>
+      </c>
+      <c r="K10" s="187" t="s">
+        <v>25</v>
+      </c>
+      <c r="L10" s="188" t="s">
+        <v>165</v>
+      </c>
+      <c r="M10" s="188" t="s">
+        <v>166</v>
+      </c>
+      <c r="N10" s="186" t="s">
+        <v>167</v>
+      </c>
+      <c r="O10" s="188" t="s">
+        <v>168</v>
+      </c>
       <c r="Q10" s="89"/>
       <c r="R10" s="89"/>
       <c r="S10" s="89"/>
@@ -8575,276 +9765,371 @@
       <c r="IP10" s="89"/>
       <c r="IQ10" s="89"/>
     </row>
-    <row r="11" spans="1:257" s="89" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A11" s="128"/>
-      <c r="B11" s="128" t="s">
+    <row r="11" spans="1:257" s="89" customFormat="1" ht="14.25">
+      <c r="A11" s="189"/>
+      <c r="B11" s="189" t="s">
         <v>81</v>
       </c>
-      <c r="C11" s="128"/>
-      <c r="D11" s="128"/>
-      <c r="E11" s="128"/>
-      <c r="F11" s="128"/>
-      <c r="G11" s="128"/>
-      <c r="H11" s="128"/>
-      <c r="I11" s="133"/>
-    </row>
-    <row r="12" spans="1:257" s="89" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A12" s="106" t="str">
+      <c r="C11" s="189"/>
+      <c r="D11" s="189"/>
+      <c r="E11" s="189"/>
+      <c r="F11" s="189"/>
+      <c r="G11" s="189"/>
+      <c r="H11" s="189"/>
+      <c r="I11" s="190"/>
+      <c r="J11" s="191"/>
+      <c r="K11" s="191"/>
+      <c r="L11" s="191"/>
+      <c r="M11" s="191"/>
+      <c r="N11" s="191"/>
+      <c r="O11" s="191"/>
+    </row>
+    <row r="12" spans="1:257" s="89" customFormat="1" ht="75">
+      <c r="A12" s="181" t="str">
         <f>"ID-" &amp; (COUNTA(A$9:A11)+1)</f>
         <v>ID-2</v>
       </c>
-      <c r="B12" s="106" t="s">
+      <c r="B12" s="181" t="s">
         <v>134</v>
       </c>
-      <c r="C12" s="106" t="s">
+      <c r="C12" s="181" t="s">
         <v>135</v>
       </c>
-      <c r="D12" s="106" t="s">
+      <c r="D12" s="181" t="s">
         <v>82</v>
       </c>
-      <c r="E12" s="106"/>
-      <c r="F12" s="106" t="s">
+      <c r="E12" s="181"/>
+      <c r="F12" s="181" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="106" t="s">
+      <c r="G12" s="181" t="s">
         <v>22</v>
       </c>
-      <c r="H12" s="106"/>
-      <c r="I12" s="106"/>
-    </row>
-    <row r="13" spans="1:257" s="89" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A13" s="106" t="str">
+      <c r="H12" s="182">
+        <v>42197</v>
+      </c>
+      <c r="I12" s="181"/>
+      <c r="J12" s="192"/>
+      <c r="K12" s="192"/>
+      <c r="L12" s="192"/>
+      <c r="M12" s="193"/>
+      <c r="N12" s="193"/>
+      <c r="O12" s="193"/>
+    </row>
+    <row r="13" spans="1:257" s="89" customFormat="1" ht="75">
+      <c r="A13" s="181" t="str">
         <f>"ID-" &amp; (COUNTA(A$9:A12)+1)</f>
         <v>ID-3</v>
       </c>
-      <c r="B13" s="106" t="s">
+      <c r="B13" s="181" t="s">
         <v>116</v>
       </c>
-      <c r="C13" s="106" t="s">
+      <c r="C13" s="181" t="s">
         <v>117</v>
       </c>
-      <c r="D13" s="106" t="s">
+      <c r="D13" s="181" t="s">
         <v>82</v>
       </c>
-      <c r="E13" s="106"/>
-      <c r="F13" s="106" t="s">
+      <c r="E13" s="181"/>
+      <c r="F13" s="181" t="s">
         <v>22</v>
       </c>
-      <c r="G13" s="106" t="s">
+      <c r="G13" s="181" t="s">
         <v>22</v>
       </c>
-      <c r="H13" s="106"/>
-      <c r="I13" s="106"/>
-    </row>
-    <row r="14" spans="1:257" s="89" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A14" s="106" t="str">
+      <c r="H13" s="182">
+        <v>42197</v>
+      </c>
+      <c r="I13" s="181"/>
+      <c r="J13" s="192"/>
+      <c r="K13" s="192"/>
+      <c r="L13" s="192"/>
+      <c r="M13" s="193"/>
+      <c r="N13" s="193"/>
+      <c r="O13" s="193"/>
+    </row>
+    <row r="14" spans="1:257" s="89" customFormat="1" ht="75">
+      <c r="A14" s="181" t="str">
         <f>"ID-" &amp; (COUNTA(A$9:A13)+1)</f>
         <v>ID-4</v>
       </c>
-      <c r="B14" s="106" t="s">
+      <c r="B14" s="181" t="s">
         <v>118</v>
       </c>
-      <c r="C14" s="106" t="s">
+      <c r="C14" s="181" t="s">
         <v>119</v>
       </c>
-      <c r="D14" s="106" t="s">
+      <c r="D14" s="181" t="s">
         <v>82</v>
       </c>
-      <c r="E14" s="106"/>
-      <c r="F14" s="106" t="s">
+      <c r="E14" s="181"/>
+      <c r="F14" s="181" t="s">
         <v>22</v>
       </c>
-      <c r="G14" s="106" t="s">
+      <c r="G14" s="181" t="s">
         <v>22</v>
       </c>
-      <c r="H14" s="106"/>
-      <c r="I14" s="106"/>
-    </row>
-    <row r="15" spans="1:257" s="89" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A15" s="106" t="str">
+      <c r="H14" s="182">
+        <v>42197</v>
+      </c>
+      <c r="I14" s="181"/>
+      <c r="J14" s="192"/>
+      <c r="K14" s="192"/>
+      <c r="L14" s="192"/>
+      <c r="M14" s="193"/>
+      <c r="N14" s="193"/>
+      <c r="O14" s="193"/>
+    </row>
+    <row r="15" spans="1:257" s="89" customFormat="1" ht="75">
+      <c r="A15" s="181" t="str">
         <f>"ID-" &amp; (COUNTA(A$9:A14)+1)</f>
         <v>ID-5</v>
       </c>
-      <c r="B15" s="106" t="s">
+      <c r="B15" s="181" t="s">
         <v>120</v>
       </c>
-      <c r="C15" s="106" t="s">
+      <c r="C15" s="181" t="s">
         <v>121</v>
       </c>
-      <c r="D15" s="106" t="s">
+      <c r="D15" s="181" t="s">
         <v>82</v>
       </c>
-      <c r="E15" s="106"/>
-      <c r="F15" s="106" t="s">
+      <c r="E15" s="181"/>
+      <c r="F15" s="181" t="s">
         <v>22</v>
       </c>
-      <c r="G15" s="106" t="s">
+      <c r="G15" s="181" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="106"/>
-      <c r="I15" s="106"/>
-    </row>
-    <row r="16" spans="1:257" s="89" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A16" s="106" t="str">
+      <c r="H15" s="182">
+        <v>42197</v>
+      </c>
+      <c r="I15" s="181"/>
+      <c r="J15" s="192"/>
+      <c r="K15" s="192"/>
+      <c r="L15" s="192"/>
+      <c r="M15" s="193"/>
+      <c r="N15" s="193"/>
+      <c r="O15" s="193"/>
+    </row>
+    <row r="16" spans="1:257" s="89" customFormat="1" ht="75">
+      <c r="A16" s="181" t="str">
         <f>"ID-" &amp; (COUNTA(A$9:A15)+1)</f>
         <v>ID-6</v>
       </c>
-      <c r="B16" s="106" t="s">
+      <c r="B16" s="181" t="s">
         <v>122</v>
       </c>
-      <c r="C16" s="106" t="s">
+      <c r="C16" s="181" t="s">
         <v>123</v>
       </c>
-      <c r="D16" s="106" t="s">
+      <c r="D16" s="181" t="s">
         <v>82</v>
       </c>
-      <c r="E16" s="106"/>
-      <c r="F16" s="106" t="s">
+      <c r="E16" s="181"/>
+      <c r="F16" s="181" t="s">
         <v>22</v>
       </c>
-      <c r="G16" s="106" t="s">
+      <c r="G16" s="181" t="s">
         <v>22</v>
       </c>
-      <c r="H16" s="106"/>
-      <c r="I16" s="106"/>
-    </row>
-    <row r="17" spans="1:10" s="89" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A17" s="106" t="str">
+      <c r="H16" s="182">
+        <v>42197</v>
+      </c>
+      <c r="I16" s="181"/>
+      <c r="J16" s="192"/>
+      <c r="K16" s="192"/>
+      <c r="L16" s="192"/>
+      <c r="M16" s="193"/>
+      <c r="N16" s="193"/>
+      <c r="O16" s="193"/>
+    </row>
+    <row r="17" spans="1:15" s="89" customFormat="1" ht="75">
+      <c r="A17" s="181" t="str">
         <f>"ID-" &amp; (COUNTA(A$9:A16)+1)</f>
         <v>ID-7</v>
       </c>
-      <c r="B17" s="106" t="s">
+      <c r="B17" s="181" t="s">
         <v>124</v>
       </c>
-      <c r="C17" s="106" t="s">
+      <c r="C17" s="181" t="s">
         <v>125</v>
       </c>
-      <c r="D17" s="106" t="s">
+      <c r="D17" s="181" t="s">
         <v>82</v>
       </c>
-      <c r="E17" s="106"/>
-      <c r="F17" s="106" t="s">
+      <c r="E17" s="181"/>
+      <c r="F17" s="181" t="s">
         <v>22</v>
       </c>
-      <c r="G17" s="106" t="s">
+      <c r="G17" s="181" t="s">
         <v>22</v>
       </c>
-      <c r="H17" s="106"/>
-      <c r="I17" s="106"/>
-    </row>
-    <row r="18" spans="1:10" ht="12.75">
-      <c r="A18" s="128"/>
-      <c r="B18" s="128" t="s">
+      <c r="H17" s="182">
+        <v>42197</v>
+      </c>
+      <c r="I17" s="181"/>
+      <c r="J17" s="192"/>
+      <c r="K17" s="192"/>
+      <c r="L17" s="192"/>
+      <c r="M17" s="193"/>
+      <c r="N17" s="193"/>
+      <c r="O17" s="193"/>
+    </row>
+    <row r="18" spans="1:15" ht="14.25">
+      <c r="A18" s="189"/>
+      <c r="B18" s="189" t="s">
         <v>136</v>
       </c>
-      <c r="C18" s="128"/>
-      <c r="D18" s="128"/>
-      <c r="E18" s="128"/>
-      <c r="F18" s="128"/>
-      <c r="G18" s="128"/>
-      <c r="H18" s="128"/>
-      <c r="I18" s="132"/>
-      <c r="J18" s="98"/>
-    </row>
-    <row r="19" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A19" s="106" t="str">
+      <c r="C18" s="189"/>
+      <c r="D18" s="189"/>
+      <c r="E18" s="189"/>
+      <c r="F18" s="189"/>
+      <c r="G18" s="189"/>
+      <c r="H18" s="189"/>
+      <c r="I18" s="194"/>
+      <c r="J18" s="191"/>
+      <c r="K18" s="191"/>
+      <c r="L18" s="191"/>
+      <c r="M18" s="191"/>
+      <c r="N18" s="191"/>
+      <c r="O18" s="191"/>
+    </row>
+    <row r="19" spans="1:15" ht="120">
+      <c r="A19" s="181" t="str">
         <f>"ID-" &amp; (COUNTA(A$9:A18)+1)</f>
         <v>ID-8</v>
       </c>
-      <c r="B19" s="106" t="s">
+      <c r="B19" s="181" t="s">
         <v>137</v>
       </c>
-      <c r="C19" s="106" t="s">
+      <c r="C19" s="181" t="s">
         <v>138</v>
       </c>
-      <c r="D19" s="106" t="s">
+      <c r="D19" s="181" t="s">
         <v>139</v>
       </c>
-      <c r="E19" s="106"/>
-      <c r="F19" s="106" t="s">
+      <c r="E19" s="181"/>
+      <c r="F19" s="181" t="s">
         <v>22</v>
       </c>
-      <c r="G19" s="106" t="s">
+      <c r="G19" s="181" t="s">
         <v>22</v>
       </c>
-      <c r="H19" s="106"/>
-      <c r="I19" s="106"/>
-      <c r="J19" s="98"/>
-    </row>
-    <row r="20" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A20" s="106" t="str">
+      <c r="H19" s="182">
+        <v>42197</v>
+      </c>
+      <c r="I19" s="181"/>
+      <c r="J19" s="192"/>
+      <c r="K19" s="192"/>
+      <c r="L19" s="192"/>
+      <c r="M19" s="193"/>
+      <c r="N19" s="193"/>
+      <c r="O19" s="193"/>
+    </row>
+    <row r="20" spans="1:15" ht="135">
+      <c r="A20" s="181" t="str">
         <f>"ID-" &amp; (COUNTA(A$9:A19)+1)</f>
         <v>ID-9</v>
       </c>
-      <c r="B20" s="106" t="s">
+      <c r="B20" s="181" t="s">
         <v>140</v>
       </c>
-      <c r="C20" s="106" t="s">
+      <c r="C20" s="181" t="s">
         <v>141</v>
       </c>
-      <c r="D20" s="106" t="s">
+      <c r="D20" s="181" t="s">
         <v>139</v>
       </c>
-      <c r="E20" s="106"/>
-      <c r="F20" s="106" t="s">
+      <c r="E20" s="181"/>
+      <c r="F20" s="181" t="s">
         <v>22</v>
       </c>
-      <c r="G20" s="106" t="s">
+      <c r="G20" s="181" t="s">
         <v>22</v>
       </c>
-      <c r="H20" s="106"/>
-      <c r="I20" s="106"/>
-      <c r="J20" s="98"/>
-    </row>
-    <row r="21" spans="1:10" ht="89.25">
-      <c r="A21" s="106" t="str">
+      <c r="H20" s="182">
+        <v>42197</v>
+      </c>
+      <c r="I20" s="181"/>
+      <c r="J20" s="192"/>
+      <c r="K20" s="192"/>
+      <c r="L20" s="192"/>
+      <c r="M20" s="193"/>
+      <c r="N20" s="193"/>
+      <c r="O20" s="193"/>
+    </row>
+    <row r="21" spans="1:15" ht="120">
+      <c r="A21" s="181" t="str">
         <f>"ID-" &amp; (COUNTA(A$9:A20)+1)</f>
         <v>ID-10</v>
       </c>
-      <c r="B21" s="106" t="s">
+      <c r="B21" s="181" t="s">
         <v>142</v>
       </c>
-      <c r="C21" s="106" t="s">
+      <c r="C21" s="181" t="s">
         <v>143</v>
       </c>
-      <c r="D21" s="106" t="s">
+      <c r="D21" s="181" t="s">
         <v>139</v>
       </c>
-      <c r="E21" s="106"/>
-      <c r="F21" s="106" t="s">
+      <c r="E21" s="181"/>
+      <c r="F21" s="181" t="s">
         <v>24</v>
       </c>
-      <c r="G21" s="106" t="s">
+      <c r="G21" s="181" t="s">
         <v>24</v>
       </c>
-      <c r="H21" s="106"/>
-      <c r="I21" s="106"/>
-      <c r="J21" s="98"/>
-    </row>
-    <row r="22" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A22" s="106" t="str">
+      <c r="H21" s="182">
+        <v>42197</v>
+      </c>
+      <c r="I21" s="181"/>
+      <c r="J21" s="192" t="s">
+        <v>162</v>
+      </c>
+      <c r="K21" s="192" t="s">
+        <v>64</v>
+      </c>
+      <c r="L21" s="192" t="s">
+        <v>152</v>
+      </c>
+      <c r="M21" s="193">
+        <v>42345</v>
+      </c>
+      <c r="N21" s="193"/>
+      <c r="O21" s="193"/>
+    </row>
+    <row r="22" spans="1:15" ht="120">
+      <c r="A22" s="181" t="str">
         <f>"ID-" &amp; (COUNTA(A$9:A21)+1)</f>
         <v>ID-11</v>
       </c>
-      <c r="B22" s="106" t="s">
+      <c r="B22" s="181" t="s">
         <v>122</v>
       </c>
-      <c r="C22" s="106" t="s">
+      <c r="C22" s="181" t="s">
         <v>144</v>
       </c>
-      <c r="D22" s="106" t="s">
+      <c r="D22" s="181" t="s">
         <v>139</v>
       </c>
-      <c r="E22" s="106"/>
-      <c r="F22" s="106" t="s">
+      <c r="E22" s="181"/>
+      <c r="F22" s="181" t="s">
         <v>22</v>
       </c>
-      <c r="G22" s="106" t="s">
+      <c r="G22" s="181" t="s">
         <v>22</v>
       </c>
-      <c r="H22" s="106"/>
-      <c r="I22" s="106"/>
-      <c r="J22" s="98"/>
+      <c r="H22" s="182">
+        <v>42197</v>
+      </c>
+      <c r="I22" s="181"/>
+      <c r="J22" s="192"/>
+      <c r="K22" s="192"/>
+      <c r="L22" s="192"/>
+      <c r="M22" s="193"/>
+      <c r="N22" s="193"/>
+      <c r="O22" s="193"/>
     </row>
   </sheetData>
   <dataConsolidate>
@@ -8876,18 +10161,42 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Calculate!$A$15:$A$20</xm:f>
+          </x14:formula1>
+          <xm:sqref>J12:J17 J19:J22</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Calculate!$A$11:$A$12</xm:f>
+          </x14:formula1>
+          <xm:sqref>K12:K17 K19:K22</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Calculate!$B$4:$B$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>L19:L22 L12:L17</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IW24"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.25" defaultRowHeight="13.5" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="15.25" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="15.125" style="117" customWidth="1"/>
     <col min="2" max="2" width="42.125" style="98" customWidth="1"/>
@@ -8898,14 +10207,14 @@
     <col min="7" max="7" width="12.75" style="98" customWidth="1"/>
     <col min="8" max="8" width="15.25" style="100" customWidth="1"/>
     <col min="9" max="9" width="15.25" style="98" customWidth="1"/>
-    <col min="10" max="10" width="13.875" style="99" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="13.875" style="99" customWidth="1"/>
     <col min="11" max="11" width="15.25" style="98" customWidth="1"/>
     <col min="12" max="16" width="15.25" style="98"/>
     <col min="17" max="17" width="0" style="98" hidden="1" customWidth="1"/>
     <col min="18" max="16384" width="15.25" style="98"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:257" ht="13.5" customHeight="1" thickBot="1">
+    <row r="1" spans="1:257" ht="14.25" thickTop="1" thickBot="1">
       <c r="A1" s="110" t="s">
         <v>48</v>
       </c>
@@ -8916,13 +10225,27 @@
       <c r="F1" s="86"/>
       <c r="G1" s="87"/>
       <c r="H1" s="88"/>
-      <c r="I1" s="89"/>
-      <c r="J1" s="89"/>
-      <c r="K1" s="89"/>
-      <c r="L1" s="89"/>
-      <c r="M1" s="89"/>
-      <c r="N1" s="89"/>
-      <c r="O1" s="89"/>
+      <c r="I1" s="167" t="s">
+        <v>158</v>
+      </c>
+      <c r="J1" s="168" t="s">
+        <v>152</v>
+      </c>
+      <c r="K1" s="168" t="s">
+        <v>153</v>
+      </c>
+      <c r="L1" s="168" t="s">
+        <v>154</v>
+      </c>
+      <c r="M1" s="168" t="s">
+        <v>155</v>
+      </c>
+      <c r="N1" s="168" t="s">
+        <v>163</v>
+      </c>
+      <c r="O1" s="169" t="s">
+        <v>150</v>
+      </c>
       <c r="P1" s="89"/>
       <c r="Q1" s="89"/>
       <c r="R1" s="89"/>
@@ -9159,30 +10482,48 @@
       <c r="IO1" s="89"/>
       <c r="IP1" s="89"/>
     </row>
-    <row r="2" spans="1:257" ht="13.5" customHeight="1">
+    <row r="2" spans="1:257" ht="15">
       <c r="A2" s="111" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="145" t="s">
+      <c r="B2" s="144" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="145"/>
-      <c r="D2" s="145"/>
-      <c r="E2" s="145"/>
-      <c r="F2" s="145"/>
-      <c r="G2" s="145"/>
+      <c r="C2" s="144"/>
+      <c r="D2" s="144"/>
+      <c r="E2" s="144"/>
+      <c r="F2" s="144"/>
+      <c r="G2" s="144"/>
       <c r="H2" s="118" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
-      <c r="O2" s="89"/>
+      <c r="I2" s="170" t="s">
+        <v>159</v>
+      </c>
+      <c r="J2" s="164">
+        <f>COUNTIFS(J12:J137,"ManhNL",L12:L137,"Open")</f>
+        <v>0</v>
+      </c>
+      <c r="K2" s="164">
+        <f>COUNTIFS(J12:J137,"ManhNL",L12:L137,"Accepted")</f>
+        <v>0</v>
+      </c>
+      <c r="L2" s="164">
+        <f>COUNTIFS(J12:J137,"ManhNL",L12:L137,"Ready for test")</f>
+        <v>0</v>
+      </c>
+      <c r="M2" s="164">
+        <f>COUNTIFS(J12:J137,"ManhNL",L12:L137,"Closed")</f>
+        <v>0</v>
+      </c>
+      <c r="N2" s="164">
+        <f>COUNTIFS(J12:J137,"ManhNL",L12:L137,"")</f>
+        <v>0</v>
+      </c>
+      <c r="O2" s="171">
+        <f t="shared" ref="O2:O7" si="0">SUM(J2:N2)</f>
+        <v>0</v>
+      </c>
       <c r="P2" s="89"/>
       <c r="Q2" s="89"/>
       <c r="R2" s="89"/>
@@ -9419,30 +10760,48 @@
       <c r="IO2" s="89"/>
       <c r="IP2" s="89"/>
     </row>
-    <row r="3" spans="1:257" ht="13.5" customHeight="1">
+    <row r="3" spans="1:257" ht="15">
       <c r="A3" s="112" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="145" t="s">
+      <c r="B3" s="144" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="145"/>
-      <c r="D3" s="145"/>
-      <c r="E3" s="145"/>
-      <c r="F3" s="145"/>
-      <c r="G3" s="145"/>
+      <c r="C3" s="144"/>
+      <c r="D3" s="144"/>
+      <c r="E3" s="144"/>
+      <c r="F3" s="144"/>
+      <c r="G3" s="144"/>
       <c r="H3" s="118" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
-      <c r="O3" s="89"/>
+      <c r="I3" s="170" t="s">
+        <v>160</v>
+      </c>
+      <c r="J3" s="164">
+        <f>COUNTIFS(J12:J137,"HuyNM",L12:L137,"Open")</f>
+        <v>0</v>
+      </c>
+      <c r="K3" s="164">
+        <f>COUNTIFS(J12:J137,"HuyNM",L12:L137,"Accepted")</f>
+        <v>0</v>
+      </c>
+      <c r="L3" s="164">
+        <f>COUNTIFS(J12:J137,"HuyNM",L12:L137,"Ready for test")</f>
+        <v>0</v>
+      </c>
+      <c r="M3" s="164">
+        <f>COUNTIFS(J12:J137,"HuyNM",L12:L137,"Closed")</f>
+        <v>0</v>
+      </c>
+      <c r="N3" s="164">
+        <f>COUNTIFS(J12:J137,"HuyNM",L12:L137,"")</f>
+        <v>0</v>
+      </c>
+      <c r="O3" s="172">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="P3" s="89"/>
       <c r="Q3" s="89"/>
       <c r="R3" s="89"/>
@@ -9679,28 +11038,48 @@
       <c r="IO3" s="89"/>
       <c r="IP3" s="89"/>
     </row>
-    <row r="4" spans="1:257" ht="13.5" customHeight="1">
+    <row r="4" spans="1:257" ht="15">
       <c r="A4" s="111" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="146" t="s">
+      <c r="B4" s="145" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="146"/>
-      <c r="D4" s="146"/>
-      <c r="E4" s="146"/>
-      <c r="F4" s="146"/>
-      <c r="G4" s="146"/>
+      <c r="C4" s="145"/>
+      <c r="D4" s="145"/>
+      <c r="E4" s="145"/>
+      <c r="F4" s="145"/>
+      <c r="G4" s="145"/>
       <c r="H4" s="118" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="89"/>
-      <c r="J4" s="90"/>
-      <c r="K4" s="89"/>
-      <c r="L4" s="89"/>
-      <c r="M4" s="89"/>
-      <c r="N4" s="89"/>
-      <c r="O4" s="89"/>
+      <c r="I4" s="170" t="s">
+        <v>161</v>
+      </c>
+      <c r="J4" s="164">
+        <f>COUNTIFS(J12:J137,"AnhDD",L12:L137,"Open")</f>
+        <v>0</v>
+      </c>
+      <c r="K4" s="164">
+        <f>COUNTIFS(J12:J137,"AnhDD",L12:L137,"Accepted")</f>
+        <v>0</v>
+      </c>
+      <c r="L4" s="164">
+        <f>COUNTIFS(J12:J137,"AnhDD",L12:L137,"Ready for test")</f>
+        <v>0</v>
+      </c>
+      <c r="M4" s="164">
+        <f>COUNTIFS(J12:J137,"AnhDD",L12:L137,"Closed")</f>
+        <v>0</v>
+      </c>
+      <c r="N4" s="164">
+        <f>COUNTIFS(J12:J137,"AnhDD",L12:L137,"")</f>
+        <v>0</v>
+      </c>
+      <c r="O4" s="172">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="P4" s="89"/>
       <c r="Q4" s="89"/>
       <c r="R4" s="89"/>
@@ -9937,7 +11316,7 @@
       <c r="IO4" s="89"/>
       <c r="IP4" s="89"/>
     </row>
-    <row r="5" spans="1:257" ht="13.5" customHeight="1">
+    <row r="5" spans="1:257" ht="15">
       <c r="A5" s="113" t="s">
         <v>22</v>
       </c>
@@ -9950,23 +11329,41 @@
       <c r="D5" s="92" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="147" t="s">
+      <c r="E5" s="146" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="147"/>
-      <c r="G5" s="147"/>
+      <c r="F5" s="146"/>
+      <c r="G5" s="146"/>
       <c r="H5" s="119" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="89"/>
-      <c r="J5" s="89" t="s">
-        <v>29</v>
-      </c>
-      <c r="K5" s="89"/>
-      <c r="L5" s="89"/>
-      <c r="M5" s="89"/>
-      <c r="N5" s="89"/>
-      <c r="O5" s="89"/>
+      <c r="I5" s="170" t="s">
+        <v>162</v>
+      </c>
+      <c r="J5" s="164">
+        <f>COUNTIFS(J12:J137,"TrungVN",L12:L137,"Open")</f>
+        <v>0</v>
+      </c>
+      <c r="K5" s="164">
+        <f>COUNTIFS(J12:J137,"TrungVN",L12:L137,"Accepted")</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="164">
+        <f>COUNTIFS(J12:J137,"TrungVN",L12:L137,"Ready for test")</f>
+        <v>0</v>
+      </c>
+      <c r="M5" s="164">
+        <f>COUNTIFS(J12:J137,"TrungVN",L12:L137,"Closed")</f>
+        <v>0</v>
+      </c>
+      <c r="N5" s="164">
+        <f>COUNTIFS(J12:J137,"TrungVN",L12:L137,"")</f>
+        <v>0</v>
+      </c>
+      <c r="O5" s="172">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="P5" s="89"/>
       <c r="Q5" s="89"/>
       <c r="R5" s="89"/>
@@ -10203,7 +11600,7 @@
       <c r="IO5" s="89"/>
       <c r="IP5" s="89"/>
     </row>
-    <row r="6" spans="1:257" ht="13.5" customHeight="1" thickBot="1">
+    <row r="6" spans="1:257" ht="15.75" thickBot="1">
       <c r="A6" s="114">
         <f>COUNTIF(F11:G183,"Pass")</f>
         <v>26</v>
@@ -10220,22 +11617,40 @@
         <f>COUNTIF(F11:G630,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="148">
+      <c r="E6" s="147">
         <f>COUNTA(A11:A187)*2</f>
         <v>26</v>
       </c>
-      <c r="F6" s="148"/>
-      <c r="G6" s="148"/>
+      <c r="F6" s="147"/>
+      <c r="G6" s="147"/>
       <c r="H6" s="93"/>
-      <c r="I6" s="89"/>
-      <c r="J6" s="89" t="s">
-        <v>27</v>
-      </c>
-      <c r="K6" s="89"/>
-      <c r="L6" s="89"/>
-      <c r="M6" s="89"/>
-      <c r="N6" s="89"/>
-      <c r="O6" s="89"/>
+      <c r="I6" s="170" t="s">
+        <v>64</v>
+      </c>
+      <c r="J6" s="164">
+        <f>COUNTIFS(J12:J137,"MaiCTP",L12:L137,"Open")</f>
+        <v>0</v>
+      </c>
+      <c r="K6" s="164">
+        <f>COUNTIFS(J12:J137,"MaiCTP",L12:L137,"Accepted")</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="164">
+        <f>COUNTIFS(J12:J137,"MaiCTP",L12:L137,"Ready for test")</f>
+        <v>0</v>
+      </c>
+      <c r="M6" s="164">
+        <f>COUNTIFS(J12:J137,"MaiCTP",L12:L137,"Closed")</f>
+        <v>0</v>
+      </c>
+      <c r="N6" s="164">
+        <f>COUNTIFS(J12:J137,"MaiCTP",L12:L137,"")</f>
+        <v>0</v>
+      </c>
+      <c r="O6" s="172">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="P6" s="89"/>
       <c r="Q6" s="89"/>
       <c r="R6" s="89"/>
@@ -10472,7 +11887,7 @@
       <c r="IO6" s="89"/>
       <c r="IP6" s="89"/>
     </row>
-    <row r="7" spans="1:257" ht="13.5" customHeight="1">
+    <row r="7" spans="1:257" ht="15">
       <c r="A7" s="129"/>
       <c r="B7" s="130"/>
       <c r="C7" s="130"/>
@@ -10481,13 +11896,33 @@
       <c r="F7" s="131"/>
       <c r="G7" s="131"/>
       <c r="H7" s="93"/>
-      <c r="I7" s="89"/>
-      <c r="J7" s="89"/>
-      <c r="K7" s="89"/>
-      <c r="L7" s="89"/>
-      <c r="M7" s="89"/>
-      <c r="N7" s="89"/>
-      <c r="O7" s="89"/>
+      <c r="I7" s="170" t="s">
+        <v>157</v>
+      </c>
+      <c r="J7" s="164">
+        <f>COUNTIFS(J12:J137,"ChinhVC",L12:L137,"Open")</f>
+        <v>0</v>
+      </c>
+      <c r="K7" s="164">
+        <f>COUNTIFS(J12:J137,"ChinhVC",L12:L137,"Accepted")</f>
+        <v>0</v>
+      </c>
+      <c r="L7" s="164">
+        <f>COUNTIFS(J12:J137,"ChinhVC",L12:L137,"Ready for test")</f>
+        <v>0</v>
+      </c>
+      <c r="M7" s="164">
+        <f>COUNTIFS(J12:J137,"ChinhVC",L12:L137,"Closed")</f>
+        <v>0</v>
+      </c>
+      <c r="N7" s="164">
+        <f>COUNTIFS(J12:J137,"ChinhVC",L12:L137,"")</f>
+        <v>0</v>
+      </c>
+      <c r="O7" s="172">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="P7" s="89"/>
       <c r="Q7" s="89"/>
       <c r="R7" s="89"/>
@@ -10724,7 +12159,7 @@
       <c r="IO7" s="89"/>
       <c r="IP7" s="89"/>
     </row>
-    <row r="8" spans="1:257" ht="13.5" customHeight="1">
+    <row r="8" spans="1:257" ht="15" thickBot="1">
       <c r="A8" s="129"/>
       <c r="B8" s="130"/>
       <c r="C8" s="130"/>
@@ -10733,13 +12168,33 @@
       <c r="F8" s="131"/>
       <c r="G8" s="131"/>
       <c r="H8" s="93"/>
-      <c r="I8" s="89"/>
-      <c r="J8" s="89"/>
-      <c r="K8" s="89"/>
-      <c r="L8" s="89"/>
-      <c r="M8" s="89"/>
-      <c r="N8" s="89"/>
-      <c r="O8" s="89"/>
+      <c r="I8" s="173" t="s">
+        <v>156</v>
+      </c>
+      <c r="J8" s="174">
+        <f>SUM(J2:J7)</f>
+        <v>0</v>
+      </c>
+      <c r="K8" s="174">
+        <f t="shared" ref="K8:O8" si="1">SUM(K2:K7)</f>
+        <v>0</v>
+      </c>
+      <c r="L8" s="174">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M8" s="174">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N8" s="174">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O8" s="174">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="P8" s="89"/>
       <c r="Q8" s="89"/>
       <c r="R8" s="89"/>
@@ -10976,7 +12431,7 @@
       <c r="IO8" s="89"/>
       <c r="IP8" s="89"/>
     </row>
-    <row r="9" spans="1:257" ht="13.5" customHeight="1">
+    <row r="9" spans="1:257" ht="13.5" thickTop="1">
       <c r="A9" s="115"/>
       <c r="B9" s="89"/>
       <c r="C9" s="89"/>
@@ -11235,7 +12690,7 @@
       <c r="IV9" s="89"/>
       <c r="IW9" s="89"/>
     </row>
-    <row r="10" spans="1:257" ht="36" customHeight="1">
+    <row r="10" spans="1:257" ht="25.5">
       <c r="A10" s="116" t="s">
         <v>30</v>
       </c>
@@ -11263,12 +12718,24 @@
       <c r="I10" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="J10" s="89"/>
-      <c r="K10" s="89"/>
-      <c r="L10" s="89"/>
-      <c r="M10" s="89"/>
-      <c r="N10" s="89"/>
-      <c r="O10" s="89"/>
+      <c r="J10" s="175" t="s">
+        <v>164</v>
+      </c>
+      <c r="K10" s="176" t="s">
+        <v>25</v>
+      </c>
+      <c r="L10" s="177" t="s">
+        <v>165</v>
+      </c>
+      <c r="M10" s="177" t="s">
+        <v>166</v>
+      </c>
+      <c r="N10" s="175" t="s">
+        <v>167</v>
+      </c>
+      <c r="O10" s="177" t="s">
+        <v>168</v>
+      </c>
       <c r="P10" s="89"/>
       <c r="Q10" s="89"/>
       <c r="R10" s="89"/>
@@ -11505,7 +12972,7 @@
       <c r="IO10" s="89"/>
       <c r="IP10" s="89"/>
     </row>
-    <row r="11" spans="1:257" s="89" customFormat="1" ht="12.75">
+    <row r="11" spans="1:257" s="89" customFormat="1">
       <c r="A11" s="128"/>
       <c r="B11" s="128" t="s">
         <v>83</v>
@@ -11516,7 +12983,13 @@
       <c r="F11" s="128"/>
       <c r="G11" s="128"/>
       <c r="H11" s="128"/>
-      <c r="I11" s="133"/>
+      <c r="I11" s="132"/>
+      <c r="J11" s="178"/>
+      <c r="K11" s="178"/>
+      <c r="L11" s="178"/>
+      <c r="M11" s="178"/>
+      <c r="N11" s="178"/>
+      <c r="O11" s="178"/>
     </row>
     <row r="12" spans="1:257" s="89" customFormat="1" ht="25.5">
       <c r="A12" s="106" t="str">
@@ -11541,6 +13014,12 @@
       </c>
       <c r="H12" s="106"/>
       <c r="I12" s="106"/>
+      <c r="J12" s="179"/>
+      <c r="K12" s="179"/>
+      <c r="L12" s="179"/>
+      <c r="M12" s="180"/>
+      <c r="N12" s="180"/>
+      <c r="O12" s="180"/>
     </row>
     <row r="13" spans="1:257" s="89" customFormat="1" ht="25.5">
       <c r="A13" s="106" t="str">
@@ -11565,6 +13044,12 @@
       </c>
       <c r="H13" s="106"/>
       <c r="I13" s="106"/>
+      <c r="J13" s="179"/>
+      <c r="K13" s="179"/>
+      <c r="L13" s="179"/>
+      <c r="M13" s="180"/>
+      <c r="N13" s="180"/>
+      <c r="O13" s="180"/>
     </row>
     <row r="14" spans="1:257" s="89" customFormat="1" ht="38.25">
       <c r="A14" s="106" t="str">
@@ -11589,6 +13074,12 @@
       </c>
       <c r="H14" s="106"/>
       <c r="I14" s="106"/>
+      <c r="J14" s="179"/>
+      <c r="K14" s="179"/>
+      <c r="L14" s="179"/>
+      <c r="M14" s="180"/>
+      <c r="N14" s="180"/>
+      <c r="O14" s="180"/>
     </row>
     <row r="15" spans="1:257" s="89" customFormat="1" ht="25.5">
       <c r="A15" s="106" t="str">
@@ -11613,6 +13104,12 @@
       </c>
       <c r="H15" s="106"/>
       <c r="I15" s="106"/>
+      <c r="J15" s="179"/>
+      <c r="K15" s="179"/>
+      <c r="L15" s="179"/>
+      <c r="M15" s="180"/>
+      <c r="N15" s="180"/>
+      <c r="O15" s="180"/>
     </row>
     <row r="16" spans="1:257" s="89" customFormat="1" ht="25.5">
       <c r="A16" s="106" t="str">
@@ -11637,8 +13134,14 @@
       </c>
       <c r="H16" s="106"/>
       <c r="I16" s="106"/>
-    </row>
-    <row r="17" spans="1:9" s="89" customFormat="1" ht="25.5">
+      <c r="J16" s="179"/>
+      <c r="K16" s="179"/>
+      <c r="L16" s="179"/>
+      <c r="M16" s="180"/>
+      <c r="N16" s="180"/>
+      <c r="O16" s="180"/>
+    </row>
+    <row r="17" spans="1:15" s="89" customFormat="1" ht="25.5">
       <c r="A17" s="106" t="str">
         <f>"ID-" &amp; (COUNTA(A$9:A16)+1)</f>
         <v>ID-7</v>
@@ -11661,8 +13164,14 @@
       </c>
       <c r="H17" s="106"/>
       <c r="I17" s="106"/>
-    </row>
-    <row r="18" spans="1:9" s="89" customFormat="1" ht="25.5">
+      <c r="J17" s="179"/>
+      <c r="K17" s="179"/>
+      <c r="L17" s="179"/>
+      <c r="M17" s="180"/>
+      <c r="N17" s="180"/>
+      <c r="O17" s="180"/>
+    </row>
+    <row r="18" spans="1:15" s="89" customFormat="1" ht="25.5">
       <c r="A18" s="106" t="str">
         <f>"ID-" &amp; (COUNTA(A$9:A17)+1)</f>
         <v>ID-8</v>
@@ -11685,8 +13194,14 @@
       </c>
       <c r="H18" s="106"/>
       <c r="I18" s="106"/>
-    </row>
-    <row r="19" spans="1:9" s="89" customFormat="1" ht="25.5">
+      <c r="J18" s="179"/>
+      <c r="K18" s="179"/>
+      <c r="L18" s="179"/>
+      <c r="M18" s="180"/>
+      <c r="N18" s="180"/>
+      <c r="O18" s="180"/>
+    </row>
+    <row r="19" spans="1:15" s="89" customFormat="1" ht="25.5">
       <c r="A19" s="106" t="str">
         <f>"ID-" &amp; (COUNTA(A$9:A18)+1)</f>
         <v>ID-9</v>
@@ -11709,8 +13224,14 @@
       </c>
       <c r="H19" s="106"/>
       <c r="I19" s="106"/>
-    </row>
-    <row r="20" spans="1:9" s="89" customFormat="1" ht="25.5">
+      <c r="J19" s="179"/>
+      <c r="K19" s="179"/>
+      <c r="L19" s="179"/>
+      <c r="M19" s="180"/>
+      <c r="N19" s="180"/>
+      <c r="O19" s="180"/>
+    </row>
+    <row r="20" spans="1:15" s="89" customFormat="1" ht="25.5">
       <c r="A20" s="106" t="str">
         <f>"ID-" &amp; (COUNTA(A$9:A19)+1)</f>
         <v>ID-10</v>
@@ -11733,8 +13254,14 @@
       </c>
       <c r="H20" s="106"/>
       <c r="I20" s="106"/>
-    </row>
-    <row r="21" spans="1:9" s="89" customFormat="1" ht="25.5">
+      <c r="J20" s="179"/>
+      <c r="K20" s="179"/>
+      <c r="L20" s="179"/>
+      <c r="M20" s="180"/>
+      <c r="N20" s="180"/>
+      <c r="O20" s="180"/>
+    </row>
+    <row r="21" spans="1:15" s="89" customFormat="1" ht="25.5">
       <c r="A21" s="106" t="str">
         <f>"ID-" &amp; (COUNTA(A$9:A20)+1)</f>
         <v>ID-11</v>
@@ -11757,8 +13284,14 @@
       </c>
       <c r="H21" s="106"/>
       <c r="I21" s="106"/>
-    </row>
-    <row r="22" spans="1:9" s="89" customFormat="1" ht="12.75">
+      <c r="J21" s="179"/>
+      <c r="K21" s="179"/>
+      <c r="L21" s="179"/>
+      <c r="M21" s="180"/>
+      <c r="N21" s="180"/>
+      <c r="O21" s="180"/>
+    </row>
+    <row r="22" spans="1:15" s="89" customFormat="1">
       <c r="A22" s="106" t="str">
         <f>"ID-" &amp; (COUNTA(A$9:A21)+1)</f>
         <v>ID-12</v>
@@ -11781,8 +13314,14 @@
       </c>
       <c r="H22" s="106"/>
       <c r="I22" s="106"/>
-    </row>
-    <row r="23" spans="1:9" s="89" customFormat="1" ht="12.75">
+      <c r="J22" s="179"/>
+      <c r="K22" s="179"/>
+      <c r="L22" s="179"/>
+      <c r="M22" s="180"/>
+      <c r="N22" s="180"/>
+      <c r="O22" s="180"/>
+    </row>
+    <row r="23" spans="1:15" s="89" customFormat="1">
       <c r="A23" s="106" t="str">
         <f>"ID-" &amp; (COUNTA(A$9:A22)+1)</f>
         <v>ID-13</v>
@@ -11805,8 +13344,14 @@
       </c>
       <c r="H23" s="106"/>
       <c r="I23" s="106"/>
-    </row>
-    <row r="24" spans="1:9" s="89" customFormat="1" ht="25.5">
+      <c r="J23" s="179"/>
+      <c r="K23" s="179"/>
+      <c r="L23" s="179"/>
+      <c r="M23" s="180"/>
+      <c r="N23" s="180"/>
+      <c r="O23" s="180"/>
+    </row>
+    <row r="24" spans="1:15" s="89" customFormat="1" ht="25.5">
       <c r="A24" s="106" t="str">
         <f>"ID-" &amp; (COUNTA(A$9:A23)+1)</f>
         <v>ID-14</v>
@@ -11829,6 +13374,12 @@
       </c>
       <c r="H24" s="106"/>
       <c r="I24" s="106"/>
+      <c r="J24" s="179"/>
+      <c r="K24" s="179"/>
+      <c r="L24" s="179"/>
+      <c r="M24" s="180"/>
+      <c r="N24" s="180"/>
+      <c r="O24" s="180"/>
     </row>
   </sheetData>
   <dataConsolidate>
@@ -11848,7 +13399,7 @@
       <formula1>$H$2:$H$5</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="WLJ12:WLQ24 WBN12:WBU24 VRR12:VRY24 VHV12:VIC24 UXZ12:UYG24 UOD12:UOK24 UEH12:UEO24 TUL12:TUS24 TKP12:TKW24 TAT12:TBA24 SQX12:SRE24 SHB12:SHI24 RXF12:RXM24 RNJ12:RNQ24 RDN12:RDU24 QTR12:QTY24 QJV12:QKC24 PZZ12:QAG24 PQD12:PQK24 PGH12:PGO24 OWL12:OWS24 OMP12:OMW24 OCT12:ODA24 NSX12:NTE24 NJB12:NJI24 MZF12:MZM24 MPJ12:MPQ24 MFN12:MFU24 LVR12:LVY24 LLV12:LMC24 LBZ12:LCG24 KSD12:KSK24 KIH12:KIO24 JYL12:JYS24 JOP12:JOW24 JET12:JFA24 IUX12:IVE24 ILB12:ILI24 IBF12:IBM24 HRJ12:HRQ24 HHN12:HHU24 GXR12:GXY24 GNV12:GOC24 GDZ12:GEG24 FUD12:FUK24 FKH12:FKO24 FAL12:FAS24 EQP12:EQW24 EGT12:EHA24 DWX12:DXE24 DNB12:DNI24 DDF12:DDM24 CTJ12:CTQ24 CJN12:CJU24 BZR12:BZY24 BPV12:BQC24 BFZ12:BGG24 AWD12:AWK24 AMH12:AMO24 ACL12:ACS24 SP12:SW24 IT12:JA24 JD11:JD24 WVF12:WVM24 WVP11:WVP24 WLT11:WLT24 WBX11:WBX24 VSB11:VSB24 VIF11:VIF24 UYJ11:UYJ24 UON11:UON24 UER11:UER24 TUV11:TUV24 TKZ11:TKZ24 TBD11:TBD24 SRH11:SRH24 SHL11:SHL24 RXP11:RXP24 RNT11:RNT24 RDX11:RDX24 QUB11:QUB24 QKF11:QKF24 QAJ11:QAJ24 PQN11:PQN24 PGR11:PGR24 OWV11:OWV24 OMZ11:OMZ24 ODD11:ODD24 NTH11:NTH24 NJL11:NJL24 MZP11:MZP24 MPT11:MPT24 MFX11:MFX24 LWB11:LWB24 LMF11:LMF24 LCJ11:LCJ24 KSN11:KSN24 KIR11:KIR24 JYV11:JYV24 JOZ11:JOZ24 JFD11:JFD24 IVH11:IVH24 ILL11:ILL24 IBP11:IBP24 HRT11:HRT24 HHX11:HHX24 GYB11:GYB24 GOF11:GOF24 GEJ11:GEJ24 FUN11:FUN24 FKR11:FKR24 FAV11:FAV24 EQZ11:EQZ24 EHD11:EHD24 DXH11:DXH24 DNL11:DNL24 DDP11:DDP24 CTT11:CTT24 CJX11:CJX24 CAB11:CAB24 BQF11:BQF24 BGJ11:BGJ24 AWN11:AWN24 AMR11:AMR24 ACV11:ACV24 SZ11:SZ24 F12:G24">
-      <formula1>$J$2:$J$6</formula1>
+      <formula1>$A$5:$D$5</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
@@ -11857,5 +13408,29 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Calculate!$B$4:$B$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>L12:L24</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Calculate!$A$11:$A$12</xm:f>
+          </x14:formula1>
+          <xm:sqref>K12:K24</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Calculate!$A$15:$A$20</xm:f>
+          </x14:formula1>
+          <xm:sqref>J12:J24</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>